<commit_message>
Initial commit for database connection and querying database
</commit_message>
<xml_diff>
--- a/hashtaglist.xlsx
+++ b/hashtaglist.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauirvin/Documents/University/Year2/205CDE/TheGramTag/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F185521B-7FB9-614A-ABD0-5B507E729BBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26860"/>
+    <workbookView xWindow="11280" yWindow="2860" windowWidth="10000" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>#theIMAGED</t>
   </si>
@@ -228,12 +230,30 @@
   </si>
   <si>
     <t>#igpodium</t>
+  </si>
+  <si>
+    <t>photography</t>
+  </si>
+  <si>
+    <t>fashion</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>wedding</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>portrait</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -256,12 +276,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -276,10 +302,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,294 +620,329 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="45.6640625" defaultRowHeight="37" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="45.6640625" style="1"/>
+    <col min="1" max="3" width="45.6640625" style="1"/>
+    <col min="4" max="4" width="49.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="45.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C22" s="2"/>
+      <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D24" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D25" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D29" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D31" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D32" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D33" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D34" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D35" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D36" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D37" s="1" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>